<commit_message>
add errors to Loss Data
</commit_message>
<xml_diff>
--- a/Loss Data.xlsx
+++ b/Loss Data.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Max_Pooling" sheetId="1" r:id="rId1"/>
     <sheet name="Mean_Pooling" sheetId="2" r:id="rId2"/>
     <sheet name="Haar_Pooling" sheetId="3" r:id="rId3"/>
     <sheet name="Daubechies 1" sheetId="4" r:id="rId4"/>
+    <sheet name="Daubechies 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Max Pooling</t>
   </si>
@@ -69,6 +70,9 @@
   </si>
   <si>
     <t>Daubechies 1 Wavelet</t>
+  </si>
+  <si>
+    <t>Daubechies 2 Wavelet Pool</t>
   </si>
 </sst>
 </file>
@@ -2973,7 +2977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3808,4 +3812,845 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G152"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0.118518888734456</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.25844028755215298</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.97935153408208797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>9.1935359370333702E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.104984720869578</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.22564912821460101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>7.2054791497416198E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.0522054356700803E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.112207256783682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>6.9109873759765503E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.4988823494520301E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6.6456201358750994E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6.13900459539325E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.78018380853563E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4.7469269817553797E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6.2025183267453599E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.9995075903331701E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3.4508933982065698E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6.5849828910335001E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.5313507475329397E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2.6471745571375101E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>6.2858304477009505E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4.0675326760931503E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.3591863612869701E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>5.8162005643149502E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4.0230917987033099E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.9799826690758901E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>4.7580351671074203E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.4620055815944399E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.75529419098274E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="1">
+        <v>1.31219953565589E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="1">
+        <v>1.1200390461591801E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="1">
+        <v>1.1120927270794299E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="1">
+        <v>9.9388285043755693E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="1">
+        <v>7.2587145829511E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="1">
+        <v>0.14551363233570999</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="1">
+        <v>5.9111644992161302E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="1">
+        <v>3.7835243191392802E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="1">
+        <v>2.99204998936968E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="1">
+        <v>2.1310142571978202E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="1">
+        <v>1.63212294815697E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="1">
+        <v>1.2942620442874499E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="1">
+        <v>1.4451074519676199E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="1">
+        <v>1.2668090087934999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="1">
+        <v>9.0266004209192795E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="1">
+        <v>8.3368543380053003E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="1">
+        <v>8.6012043578927305E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="1">
+        <v>7.8129862432257495E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="1">
+        <v>5.5111141798054502E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="1">
+        <v>5.9492031916833603E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="1">
+        <v>9.0007804224809099E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="1">
+        <v>4.0787466728007302E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="1">
+        <v>3.2238655067846698E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="1">
+        <v>1.9821564649314699E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="1">
+        <v>1.6662514676784399E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="1">
+        <v>1.29473182623412E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="1">
+        <v>1.0601431381550499E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="1">
+        <v>9.2169901834292401E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="1">
+        <v>9.6331711501641496E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="1">
+        <v>7.8392888795995805E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="1">
+        <v>7.25142135127896E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="1">
+        <v>7.5658526211530601E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="1">
+        <v>4.7657113462027103E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="1">
+        <v>5.7609170752958199E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="1">
+        <v>4.8699365168316704E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="1">
+        <v>6.53711578052006E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="1">
+        <v>3.1334481704749902E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="1">
+        <v>2.2455087472134299E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="1">
+        <v>1.7763515870261901E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="1">
+        <v>1.30109048084664E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="1">
+        <v>1.01374058630101E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G54" s="1">
+        <v>1.0339199105630499E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G55" s="1">
+        <v>7.9822487420968691E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="1">
+        <v>6.9490454491861701E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="1">
+        <v>6.48667464289989E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G58" s="1">
+        <v>5.4185561041138102E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G59" s="1">
+        <v>4.9283674505467799E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G60" s="1">
+        <v>4.3952306281774597E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G61" s="1">
+        <v>5.1771505798985304E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="1">
+        <v>4.6993849400464001E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G63" s="1">
+        <v>5.7384184685076001E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="1">
+        <v>2.6057927786792799E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G65" s="1">
+        <v>1.64945693634382E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="1">
+        <v>1.3659705746167801E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="1">
+        <v>1.33717032904051E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G68" s="1">
+        <v>9.3748556727519406E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G69" s="1">
+        <v>5.6827760620638303E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G70" s="1">
+        <v>7.6376197748934897E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G71" s="1">
+        <v>5.0414235420182798E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G72" s="1">
+        <v>6.26401924883138E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G73" s="1">
+        <v>5.4376810451900797E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G74" s="1">
+        <v>5.7931017815321898E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G75" s="1">
+        <v>4.71081483898886E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G76" s="1">
+        <v>5.2650483801038204E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G77" s="1">
+        <v>3.8080647569533701E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G78" s="1">
+        <v>4.7724747806241599E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G79" s="1">
+        <v>2.7708234520099299E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G80" s="1">
+        <v>1.53716380970885E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G81" s="1">
+        <v>1.47633205972671E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G82" s="1">
+        <v>1.05468871622871E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G83" s="1">
+        <v>8.8859802343595404E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G84" s="1">
+        <v>7.4596171723624698E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G85" s="1">
+        <v>6.7478948402214002E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G86" s="1">
+        <v>6.2320374135740597E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G87" s="1">
+        <v>4.8361889354348597E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G88" s="1">
+        <v>3.9209042705065297E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G89" s="1">
+        <v>3.9000713419164198E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G90" s="1">
+        <v>3.87807521891438E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G91" s="1">
+        <v>2.7967121772736101E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G92" s="1">
+        <v>3.0277300929664199E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G93" s="1">
+        <v>3.1508575959371503E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G94" s="1">
+        <v>1.8862243405077399E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G95" s="1">
+        <v>1.44282620920683E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G96" s="1">
+        <v>9.3793625535509503E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G97" s="1">
+        <v>9.9430322631639603E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G98" s="1">
+        <v>8.4442368386997493E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G99" s="1">
+        <v>6.3207181814132398E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G100" s="1">
+        <v>5.2208010677689898E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G101" s="1">
+        <v>5.1114476304980399E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G102" s="1">
+        <v>4.0878284080476997E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G103" s="1">
+        <v>4.0237604300998302E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G104" s="1">
+        <v>4.8296025737400603E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G105" s="1">
+        <v>3.8948292947477599E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G106" s="1">
+        <v>3.8180979665006398E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G107" s="1">
+        <v>3.3394155984182699E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G108" s="1">
+        <v>4.33947467824254E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G109" s="1">
+        <v>2.02077387195587E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G110" s="1">
+        <v>1.4305693949107001E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G111" s="1">
+        <v>1.03744820501732E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G112" s="1">
+        <v>7.20133157043176E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G113" s="1">
+        <v>6.80370455064974E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G114" s="1">
+        <v>6.8350375830504304E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G115" s="1">
+        <v>4.92987122356123E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G116" s="1">
+        <v>4.0279746289463196E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G117" s="1">
+        <v>4.3603527689494697E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G118" s="1">
+        <v>4.08003955701458E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G119" s="1">
+        <v>2.3583837897785398E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G120" s="1">
+        <v>4.0358569574113603E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G121" s="1">
+        <v>2.9804395179129301E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G122" s="1">
+        <v>2.0375276977914699E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G123" s="1">
+        <v>3.5697547854201303E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G124" s="1">
+        <v>1.6620434403969299E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G125" s="1">
+        <v>1.52046631484129E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G126" s="1">
+        <v>9.6827560755977093E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G127" s="1">
+        <v>8.7216659296499698E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G128" s="1">
+        <v>7.0812287622975499E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G129" s="1">
+        <v>5.8527926044084399E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G130" s="1">
+        <v>3.8770302490118598E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G131" s="1">
+        <v>5.4970938600570401E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G132" s="1">
+        <v>4.23447930745003E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G133" s="1">
+        <v>3.4140525007675302E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G134" s="1">
+        <v>3.5522545322082401E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G135" s="1">
+        <v>3.37671854074016E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G136" s="1">
+        <v>2.41628896543608E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G137" s="1">
+        <v>2.8248793796702199E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G138" s="1">
+        <v>3.5172809490859602E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G139" s="1">
+        <v>1.8557333332272E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G140" s="1">
+        <v>1.2748952880187899E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G141" s="1">
+        <v>8.5014486425086608E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G142" s="1">
+        <v>5.0870060992989899E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G143" s="1">
+        <v>4.3282612268538299E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G144" s="1">
+        <v>5.1470129796826599E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G145" s="1">
+        <v>3.9102148453995797E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G146" s="1">
+        <v>3.4099061785345299E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G147" s="1">
+        <v>3.3402478935726301E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G148" s="1">
+        <v>3.3361872397687699E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G149" s="1">
+        <v>3.0353839799962998E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G150" s="1">
+        <v>2.8238339051452998E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G151" s="1">
+        <v>2.9898452971357401E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G152" s="1">
+        <v>2.6842215685221799E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Do 5 wavelet pooling tests
Haar, Daubechies 1, 2, Coiflet 1
</commit_message>
<xml_diff>
--- a/Loss Data.xlsx
+++ b/Loss Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec\Documents\GitHub\DSGA_1013_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D551E8-B03C-4AB1-B8DB-EBBB1C50A4C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AC89A9-E23F-457E-83D7-8ADF23A2361C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Max Pooling</t>
   </si>
@@ -108,6 +108,81 @@
   </si>
   <si>
     <t>Max Pool</t>
+  </si>
+  <si>
+    <t>Mean Pool</t>
+  </si>
+  <si>
+    <t>Haar Pool</t>
+  </si>
+  <si>
+    <t>[0.4552,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5396,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5741,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5826,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5856,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5969,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5941,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5966,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6013,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6008]</t>
+  </si>
+  <si>
+    <t>Db2</t>
+  </si>
+  <si>
+    <t>Db1</t>
+  </si>
+  <si>
+    <t>[0.4822,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5233,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5514,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5728,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5753,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5759,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5873,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5888,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5927,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5833]</t>
+  </si>
+  <si>
+    <t>Coif1</t>
   </si>
 </sst>
 </file>
@@ -4698,67 +4773,236 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B052E035-1517-46FA-AA1B-B3DF8C40A41D}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C23:C24"/>
+      <selection activeCell="K2" sqref="K2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="5" max="5" width="16.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="C2" s="6">
+        <v>0.41370000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.48780000000000001</v>
+      </c>
+      <c r="G2">
+        <v>0.48609999999999998</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="C3">
+        <v>0.51980000000000004</v>
+      </c>
+      <c r="E3">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="G3">
+        <v>0.52149999999999996</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="C4">
+        <v>0.55889999999999995</v>
+      </c>
+      <c r="E4">
+        <v>0.58009999999999995</v>
+      </c>
+      <c r="G4">
+        <v>0.58209999999999995</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="C5">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.59040000000000004</v>
+      </c>
+      <c r="G5">
+        <v>0.58819999999999995</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="C6">
+        <v>0.60040000000000004</v>
+      </c>
+      <c r="E6">
+        <v>0.59750000000000003</v>
+      </c>
+      <c r="G6">
+        <v>0.5907</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="C7">
+        <v>0.59970000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.59909999999999997</v>
+      </c>
+      <c r="G7">
+        <v>0.59340000000000004</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="C8">
+        <v>0.6089</v>
+      </c>
+      <c r="E8">
+        <v>0.5998</v>
+      </c>
+      <c r="G8">
+        <v>0.60929999999999995</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="C9">
+        <v>0.60389999999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.60760000000000003</v>
+      </c>
+      <c r="G9">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="C10">
+        <v>0.62070000000000003</v>
+      </c>
+      <c r="E10">
+        <v>0.60040000000000004</v>
+      </c>
+      <c r="G10">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="6" t="s">
         <v>23</v>
+      </c>
+      <c r="C11">
+        <v>0.61570000000000003</v>
+      </c>
+      <c r="E11">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.60650000000000004</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish CIFAR accuracy tests
</commit_message>
<xml_diff>
--- a/Loss Data.xlsx
+++ b/Loss Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec\Documents\GitHub\DSGA_1013_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AC89A9-E23F-457E-83D7-8ADF23A2361C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026229F9-8CD5-4427-A6ED-1619DC950A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Max_Pooling" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Daubechies 1" sheetId="4" r:id="rId4"/>
     <sheet name="Daubechies 2" sheetId="5" r:id="rId5"/>
     <sheet name="CIFAR Pooling Accuracies" sheetId="6" r:id="rId6"/>
+    <sheet name="CIFAR Pooling Accuracy slow" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="153">
   <si>
     <t>Max Pooling</t>
   </si>
@@ -183,6 +184,315 @@
   </si>
   <si>
     <t>Coif1</t>
+  </si>
+  <si>
+    <t>Haar</t>
+  </si>
+  <si>
+    <t>[0.3944,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4522,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4885,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5101,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5279,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5448,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.556,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5626,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5808,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5793,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5866,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5902,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5993,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6065,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6093,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6089,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6139,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6104,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6112]</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>[0.375,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4465,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4698,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4962,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5191,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5291,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5519,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5575,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5704,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5725,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5824,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6018,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5955,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6061,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6046,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6162,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6178,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6152,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6215,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6213]</t>
+  </si>
+  <si>
+    <t>db2</t>
+  </si>
+  <si>
+    <t>[0.378,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4427,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4791,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4925,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5166,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5223,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5368,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5481,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5602,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5621,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.572,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5815,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.587,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5874,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5986,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5989,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6074,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6011,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6094,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6077]</t>
+  </si>
+  <si>
+    <t>coif1</t>
+  </si>
+  <si>
+    <t>[0.3868,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4417,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.467,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.485,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5022,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5212,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5282,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5363,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.554,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5613,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5709,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5788,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5766,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5722,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5805,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5886,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5922,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.599,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5978,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5907]</t>
+  </si>
+  <si>
+    <t>bior1.1</t>
+  </si>
+  <si>
+    <t>[0.3939,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4515,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4813,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4995,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5072,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5313,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5507,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5503,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5619,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5642,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5719,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5743,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5895,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5937,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6059,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6041,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6105,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6109,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6113]</t>
   </si>
 </sst>
 </file>
@@ -4775,7 +5085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B052E035-1517-46FA-AA1B-B3DF8C40A41D}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:K11"/>
     </sheetView>
   </sheetViews>
@@ -5009,4 +5319,377 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDC86A7-95F6-4F6B-A374-D92F5E2E56E5}">
+  <dimension ref="B1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="2:10">
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10">
+      <c r="B2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>